<commit_message>
Replaced pi with h
</commit_message>
<xml_diff>
--- a/database/sidis/expdata/9011.xlsx
+++ b/database/sidis/expdata/9011.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fafd12/GIT/jam3d/database/sidis/expdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/physicsstudentresearch/Documents/jam3d/database/sidis/expdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A00C307F-7031-B148-A2A2-977AAF6D27F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0822C7C-6A6C-C840-B915-880A14F9F3A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2320" yWindow="2560" windowWidth="28040" windowHeight="17440" xr2:uid="{D2E5834A-E2D0-644B-94F2-5F0D9153EBFE}"/>
+    <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="16500" xr2:uid="{D2E5834A-E2D0-644B-94F2-5F0D9153EBFE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -75,14 +75,14 @@
     <t>dependence</t>
   </si>
   <si>
-    <t>pi+</t>
+    <t>h+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -436,12 +436,12 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K11"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -482,7 +482,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0.22</v>
       </c>
@@ -523,7 +523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0.27</v>
       </c>
@@ -564,7 +564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>0.32</v>
       </c>
@@ -605,7 +605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0.37</v>
       </c>
@@ -646,7 +646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0.42</v>
       </c>
@@ -687,7 +687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0.47</v>
       </c>
@@ -728,7 +728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0.55000000000000004</v>
       </c>
@@ -769,7 +769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>0.65</v>
       </c>
@@ -810,7 +810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>0.75</v>
       </c>
@@ -851,7 +851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>0.88</v>
       </c>

</xml_diff>